<commit_message>
Repositioned cursor for template
</commit_message>
<xml_diff>
--- a/fms_core/static/submission_templates/Sample_submission_v0.10.xlsx
+++ b/fms_core/static/submission_templates/Sample_submission_v0.10.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="SampleSubmission" sheetId="1" state="visible" r:id="rId2"/>
@@ -56,7 +56,7 @@
     <t xml:space="preserve">Naming Rules</t>
   </si>
   <si>
-    <t xml:space="preserve">- Only use the follwin caracters for Sample name and Barcode: a-z, A-Z, 0-9, period (.), dash (-), underscore ( _ )</t>
+    <t xml:space="preserve">- Only use the following characters for Sample name and Barcode: a-z, A-Z, 0-9, period (.), dash (-), underscore ( _ )</t>
   </si>
   <si>
     <t xml:space="preserve">#</t>
@@ -1653,11 +1653,11 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.26"/>
@@ -1670,7 +1670,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="17.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="13"/>
@@ -17485,14 +17485,14 @@
   </sheetPr>
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="9.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.13"/>

</xml_diff>

<commit_message>
fixed an error with coord validation formula.
</commit_message>
<xml_diff>
--- a/fms_core/static/submission_templates/Sample_submission_v0.10.xlsx
+++ b/fms_core/static/submission_templates/Sample_submission_v0.10.xlsx
@@ -1654,10 +1654,10 @@
   <dimension ref="A1:X1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.26"/>
@@ -1812,7 +1812,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
         <v>1</v>
       </c>
@@ -1840,7 +1840,7 @@
       <c r="W8" s="8"/>
       <c r="X8" s="8"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
         <v>2</v>
       </c>
@@ -1868,7 +1868,7 @@
       <c r="W9" s="8"/>
       <c r="X9" s="8"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="n">
         <v>3</v>
       </c>
@@ -1896,7 +1896,7 @@
       <c r="W10" s="8"/>
       <c r="X10" s="8"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="n">
         <v>4</v>
       </c>
@@ -1924,7 +1924,7 @@
       <c r="W11" s="8"/>
       <c r="X11" s="8"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="n">
         <v>5</v>
       </c>
@@ -1952,7 +1952,7 @@
       <c r="W12" s="8"/>
       <c r="X12" s="8"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="n">
         <v>6</v>
       </c>
@@ -1980,7 +1980,7 @@
       <c r="W13" s="8"/>
       <c r="X13" s="8"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="n">
         <v>7</v>
       </c>
@@ -2008,7 +2008,7 @@
       <c r="W14" s="8"/>
       <c r="X14" s="8"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="n">
         <v>8</v>
       </c>
@@ -2036,7 +2036,7 @@
       <c r="W15" s="8"/>
       <c r="X15" s="8"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="n">
         <v>9</v>
       </c>
@@ -2064,7 +2064,7 @@
       <c r="W16" s="8"/>
       <c r="X16" s="8"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="n">
         <v>10</v>
       </c>
@@ -2092,7 +2092,7 @@
       <c r="W17" s="8"/>
       <c r="X17" s="8"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="n">
         <v>11</v>
       </c>
@@ -2120,7 +2120,7 @@
       <c r="W18" s="8"/>
       <c r="X18" s="8"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="n">
         <v>12</v>
       </c>
@@ -2148,7 +2148,7 @@
       <c r="W19" s="8"/>
       <c r="X19" s="8"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="n">
         <v>13</v>
       </c>
@@ -17450,10 +17450,6 @@
       <formula1>Index!$F$2:$F$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" prompt="Coordinate" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L8:L391" type="list">
-      <formula1>IF(OR(H10="Tube",H10="96-well plate"),Index!$A$2:$A$97,IF(H10="384-well plate",Index!$B$2:$B$385,""))</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B8:B391" type="list">
       <formula1>Index!$C$2:$C$8</formula1>
       <formula2>0</formula2>
@@ -17464,6 +17460,10 @@
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="U8:U391" type="list">
       <formula1>Index!$H$2:$H$11</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" prompt="Coordinate" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L8:L391" type="list">
+      <formula1>IF(OR(H8="Tube",H8="96-well plate"),Index!$A$2:$A$97,IF(H8="384-well plate",Index!$B$2:$B$385,""))</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -17489,7 +17489,7 @@
       <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="9.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.06"/>

</xml_diff>

<commit_message>
Correct validation of template. Prevent Traceback when not in DEBUG.
</commit_message>
<xml_diff>
--- a/fms_core/static/submission_templates/Sample_submission_v0.10.xlsx
+++ b/fms_core/static/submission_templates/Sample_submission_v0.10.xlsx
@@ -1660,7 +1660,7 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.26"/>
@@ -17466,7 +17466,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" prompt="Coordinate" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L8:L391" type="list">
-      <formula1>IF(OR(#REF!="Tube",#REF!="96-well plate"),Index!$A$2:$A$97,IF(#REF!="384-well plate",Index!$B$2:$B$385,""))</formula1>
+      <formula1>IF(OR($H8="Tube",$H8="96-well plate"),Index!$A$2:$A$97,IF($H8="384-well plate",Index!$B$2:$B$385,""))</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -17492,7 +17492,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="9.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.06"/>

</xml_diff>